<commit_message>
changed the username and password
</commit_message>
<xml_diff>
--- a/DataSheet/DataSheet_Sample_Selenium.xlsx
+++ b/DataSheet/DataSheet_Sample_Selenium.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F36EA82-923B-417E-A965-7EB962303385}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE8DF60-D010-40B4-A4FA-3D56E17C4863}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4392" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>WebBrowser</t>
   </si>
@@ -34,10 +34,7 @@
     <t>Password</t>
   </si>
   <si>
-    <t>homeacc0118@gmail.com</t>
-  </si>
-  <si>
-    <t>sidniki118</t>
+    <t>***</t>
   </si>
 </sst>
 </file>
@@ -385,7 +382,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>